<commit_message>
output view build stats
</commit_message>
<xml_diff>
--- a/graph_expr/output/goodcol_outputs- Email_lb20_lb20_cyc_m_q7/Email_lb20_lb20_cyc_m_q7__simgrBYVIEWS_newcols.xlsx
+++ b/graph_expr/output/goodcol_outputs- Email_lb20_lb20_cyc_m_q7/Email_lb20_lb20_cyc_m_q7__simgrBYVIEWS_newcols.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t xml:space="preserve">*****************************************************</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">Average of 3 runs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">once you prefilter, there’s less to filter by simulation. Prefiltering is fast but not as efficient as reducing. Prefilt helps sim filtering very much</t>
   </si>
 </sst>
 </file>
@@ -218,12 +221,13 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,13 +245,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -259,6 +256,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -266,20 +264,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -339,8 +323,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,47 +336,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,11 +387,11 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.046875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -838,13 +814,14 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="10"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="2" width="11.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="10"/>
   </cols>
@@ -956,31 +933,31 @@
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="n">
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>0.02</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="4" t="n">
         <v>0.03</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="7" t="n">
         <v>0.04</v>
       </c>
-      <c r="G4" s="8" t="n">
-        <v>53443</v>
-      </c>
-      <c r="H4" s="8" t="n">
+      <c r="G4" s="4" t="n">
+        <v>53443</v>
+      </c>
+      <c r="H4" s="4" t="n">
         <v>685</v>
       </c>
-      <c r="I4" s="8" t="n">
-        <v>50083</v>
-      </c>
-      <c r="J4" s="8" t="n">
+      <c r="I4" s="4" t="n">
+        <v>50083</v>
+      </c>
+      <c r="J4" s="4" t="n">
         <v>23681</v>
       </c>
       <c r="K4" s="6" t="n">
@@ -1002,7 +979,7 @@
       <c r="E5" s="2" t="n">
         <v>0.02</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="8" t="n">
         <v>2.6</v>
       </c>
       <c r="G5" s="2" t="n">
@@ -1036,7 +1013,7 @@
       <c r="E6" s="2" t="n">
         <v>0.11</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="8" t="n">
         <v>2.17</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -1070,7 +1047,7 @@
       <c r="E7" s="2" t="n">
         <v>0.02</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="8" t="n">
         <v>0.67</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -1163,19 +1140,19 @@
       <c r="E11" s="6" t="n">
         <v>0.02</v>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="F11" s="9" t="n">
         <v>2.23</v>
       </c>
-      <c r="G11" s="12" t="n">
+      <c r="G11" s="10" t="n">
         <v>53443</v>
       </c>
       <c r="H11" s="6" t="n">
         <v>685</v>
       </c>
-      <c r="I11" s="12" t="n">
-        <v>50083</v>
-      </c>
-      <c r="J11" s="12" t="n">
+      <c r="I11" s="10" t="n">
+        <v>50083</v>
+      </c>
+      <c r="J11" s="10" t="n">
         <v>23681</v>
       </c>
       <c r="K11" s="6" t="n">
@@ -1199,19 +1176,19 @@
       <c r="E12" s="6" t="n">
         <v>0.05</v>
       </c>
-      <c r="F12" s="11" t="n">
+      <c r="F12" s="9" t="n">
         <v>1.64</v>
       </c>
-      <c r="G12" s="12" t="n">
-        <v>53443</v>
-      </c>
-      <c r="H12" s="12" t="n">
+      <c r="G12" s="10" t="n">
+        <v>53443</v>
+      </c>
+      <c r="H12" s="10" t="n">
         <v>10342</v>
       </c>
-      <c r="I12" s="12" t="n">
-        <v>50083</v>
-      </c>
-      <c r="J12" s="12" t="n">
+      <c r="I12" s="10" t="n">
+        <v>50083</v>
+      </c>
+      <c r="J12" s="10" t="n">
         <v>1517827</v>
       </c>
       <c r="K12" s="6" t="n">
@@ -1235,19 +1212,19 @@
       <c r="E13" s="6" t="n">
         <v>0.01</v>
       </c>
-      <c r="F13" s="11" t="n">
+      <c r="F13" s="9" t="n">
         <v>0.57</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="G13" s="10" t="n">
         <v>53443</v>
       </c>
       <c r="H13" s="6" t="n">
         <v>685</v>
       </c>
-      <c r="I13" s="12" t="n">
-        <v>50083</v>
-      </c>
-      <c r="J13" s="12" t="n">
+      <c r="I13" s="10" t="n">
+        <v>50083</v>
+      </c>
+      <c r="J13" s="10" t="n">
         <v>23681</v>
       </c>
       <c r="K13" s="6" t="n">
@@ -1262,7 +1239,9 @@
     </row>
     <row r="16" s="4" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>

</xml_diff>